<commit_message>
*  Author: freddy  *  Created on: Thu 20 Oct 2022 12:24:33 PM MDT
</commit_message>
<xml_diff>
--- a/inputs/test_example.xlsx
+++ b/inputs/test_example.xlsx
@@ -1,231 +1,230 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher.Wilson\Documents\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Redbock\Desktop\bmrn-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4D5547-15A1-4647-9EEA-DA0F8B10E636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C0634E-658B-402B-913A-42958C678AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="21600" windowHeight="11325" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tmp" sheetId="1" r:id="rId1"/>
+    <sheet name="Instruction" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Entry" sheetId="2" r:id="rId2"/>
+    <sheet name="Example" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="21">
-  <si>
-    <t>Non-Wild Type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="50">
+  <si>
+    <t>In cell B1, please record the label for your endpoint or biomarker with unit</t>
+  </si>
+  <si>
+    <t>This is the label that will be displayed on the y-axis of the output graphs.</t>
+  </si>
+  <si>
+    <t>In cell D1, please record LLOQ if there are BLQ in your data</t>
+  </si>
+  <si>
+    <t>This should be a number only, no units.</t>
+  </si>
+  <si>
+    <t>Grey cells are fixed text that cannot be changed.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>This describes the type of model used in the study (i.e. the genotype, genetic background or disease model used).</t>
+  </si>
+  <si>
+    <t>Treatment group name</t>
+  </si>
+  <si>
+    <t>This describes the treatment, if any, that was administered to the subjects during the study. It will be included as text on the output graph.</t>
+  </si>
+  <si>
+    <t>Subject ID</t>
+  </si>
+  <si>
+    <t>This is the identifier for each subject (e.g. mouse) included in the study.</t>
+  </si>
+  <si>
+    <t>Techical Replicate ID</t>
+  </si>
+  <si>
+    <t>If there are replicate measures for a subject, enter the replicate IDs here. This field can be left blank if there are no techinical replicates.</t>
+  </si>
+  <si>
+    <t>Dose with units</t>
+  </si>
+  <si>
+    <t>This is the dosing information. It will be included as text on the output graphs. For subjects that are not dosed, leave blank.</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>This is the baseline measurement of your endpoint or biomarker (numbers only, do not include units). This field can be left blank if there is not baseline for the study.</t>
+  </si>
+  <si>
+    <t>Time1, Time2….</t>
+  </si>
+  <si>
+    <t>Replace the text in these boxes with the time points for your study (including units). Input the endpoint or biomarker values for each subject in the rows below.</t>
+  </si>
+  <si>
+    <t>"Example" sheet</t>
+  </si>
+  <si>
+    <t>Review this sheet to see an example of what the data input looks like.</t>
+  </si>
+  <si>
+    <t>Treatment Group Name</t>
+  </si>
+  <si>
+    <t>SubjectID</t>
+  </si>
+  <si>
+    <t>Time1 (free text)</t>
+  </si>
+  <si>
+    <t>Time2 (free text)</t>
+  </si>
+  <si>
+    <t>Time3 (free text)</t>
+  </si>
+  <si>
+    <t>Time4 (free text)</t>
+  </si>
+  <si>
+    <t>Time5 (free text)</t>
+  </si>
+  <si>
+    <t>Wild type</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease </t>
+  </si>
+  <si>
+    <t>Negative Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postive Control </t>
+  </si>
+  <si>
+    <t>Trt</t>
+  </si>
+  <si>
+    <t>creatine kinase (ng/ml)</t>
+  </si>
+  <si>
+    <t>Technical Replicate ID</t>
+  </si>
+  <si>
+    <t>BMN000</t>
+  </si>
+  <si>
+    <t>Dose</t>
+  </si>
+  <si>
+    <t>week 2</t>
+  </si>
+  <si>
+    <t>week 4</t>
+  </si>
+  <si>
+    <t>week 5</t>
+  </si>
+  <si>
+    <t>week 8</t>
+  </si>
+  <si>
+    <t>week 10</t>
+  </si>
+  <si>
+    <t>week 12</t>
+  </si>
+  <si>
+    <t>week 15</t>
+  </si>
+  <si>
+    <t>Diseased</t>
+  </si>
+  <si>
+    <t>100 mg/vg</t>
+  </si>
+  <si>
+    <t>200 mg/vg</t>
+  </si>
+  <si>
+    <t>300 mg/vg</t>
   </si>
   <si>
     <t>Wild Type</t>
-  </si>
-  <si>
-    <t>In cell B1, please record the label for your endpoint or biomarker with unit</t>
-  </si>
-  <si>
-    <t>creatine kinase (ng/ml)</t>
-  </si>
-  <si>
-    <t>In cell D1, please record LLOQ if there are BLQ in your data</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Treatment Group Name</t>
-  </si>
-  <si>
-    <t>SubjectID</t>
-  </si>
-  <si>
-    <t>Technical Replicate ID</t>
-  </si>
-  <si>
-    <t>Dose</t>
-  </si>
-  <si>
-    <t>Baseline</t>
-  </si>
-  <si>
-    <t>Day 1</t>
-  </si>
-  <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>e13</t>
-  </si>
-  <si>
-    <t>e13 empty-NP</t>
-  </si>
-  <si>
-    <t>e13 no rap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -236,21 +235,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,185 +245,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -445,222 +258,128 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFE7E6E6"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -969,103 +688,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="6" customWidth="1"/>
+    <col min="3" max="11" width="9.140625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:M63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="6" customWidth="1"/>
+    <col min="5" max="6" width="10.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="6" customWidth="1"/>
+    <col min="8" max="11" width="9.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3">
+      <c r="D1" s="8">
         <v>20</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="B3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1073,8 +1017,8 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>100</v>
+      <c r="E4" t="s">
+        <v>46</v>
       </c>
       <c r="F4">
         <v>0.941074597238576</v>
@@ -1101,12 +1045,12 @@
         <v>3.43253215339353</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1114,8 +1058,8 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>100</v>
+      <c r="E5" t="s">
+        <v>46</v>
       </c>
       <c r="F5">
         <v>0.941074597238576</v>
@@ -1142,12 +1086,12 @@
         <v>3.0184423143574302</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1155,8 +1099,8 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>100</v>
+      <c r="E6" t="s">
+        <v>46</v>
       </c>
       <c r="F6">
         <v>0.69178120368932094</v>
@@ -1183,12 +1127,12 @@
         <v>4.8149585611572299</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1196,8 +1140,8 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7">
-        <v>100</v>
+      <c r="E7" t="s">
+        <v>46</v>
       </c>
       <c r="F7">
         <v>0.69178120368932094</v>
@@ -1224,12 +1168,12 @@
         <v>2.6520158468147401</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1237,8 +1181,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>100</v>
+      <c r="E8" t="s">
+        <v>46</v>
       </c>
       <c r="F8">
         <v>1.88351526788246</v>
@@ -1265,12 +1209,12 @@
         <v>1.5259770345946699</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1278,8 +1222,8 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9">
-        <v>100</v>
+      <c r="E9" t="s">
+        <v>46</v>
       </c>
       <c r="F9">
         <v>1.88351526788246</v>
@@ -1306,12 +1250,12 @@
         <v>4.45300214355722</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -1319,8 +1263,8 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>100</v>
+      <c r="E10" t="s">
+        <v>46</v>
       </c>
       <c r="F10">
         <v>-0.39390612148918602</v>
@@ -1347,12 +1291,12 @@
         <v>1.80582866758543</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -1360,8 +1304,8 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>100</v>
+      <c r="E11" t="s">
+        <v>46</v>
       </c>
       <c r="F11">
         <v>-0.39390612148918602</v>
@@ -1388,12 +1332,12 @@
         <v>5.1027477154200698</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1401,8 +1345,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>100</v>
+      <c r="E12" t="s">
+        <v>46</v>
       </c>
       <c r="F12">
         <v>7.53786393623887E-2</v>
@@ -1429,12 +1373,12 @@
         <v>3.77085435949768</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -1442,8 +1386,8 @@
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13">
-        <v>100</v>
+      <c r="E13" t="s">
+        <v>46</v>
       </c>
       <c r="F13">
         <v>7.53786393623887E-2</v>
@@ -1470,12 +1414,12 @@
         <v>4.2211279298530604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -1483,8 +1427,8 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>200</v>
+      <c r="E14" t="s">
+        <v>47</v>
       </c>
       <c r="F14">
         <v>0.87663252186751905</v>
@@ -1511,12 +1455,12 @@
         <v>2.3826694512861502</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -1524,8 +1468,9 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15">
-        <v>200</v>
+      <c r="E15" t="str">
+        <f>E14</f>
+        <v>200 mg/vg</v>
       </c>
       <c r="F15">
         <v>0.87663252186751905</v>
@@ -1552,12 +1497,12 @@
         <v>2.8488228773036499</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>7</v>
@@ -1565,8 +1510,9 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>200</v>
+      <c r="E16" t="str">
+        <f t="shared" ref="E16:E23" si="0">E15</f>
+        <v>200 mg/vg</v>
       </c>
       <c r="F16">
         <v>1.1232273718449</v>
@@ -1593,12 +1539,12 @@
         <v>4.1180718475959299</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -1606,8 +1552,9 @@
       <c r="D17">
         <v>2</v>
       </c>
-      <c r="E17">
-        <v>200</v>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>200 mg/vg</v>
       </c>
       <c r="F17">
         <v>1.1232273718449</v>
@@ -1634,12 +1581,12 @@
         <v>2.2341203226563899</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -1647,8 +1594,9 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18">
-        <v>200</v>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>200 mg/vg</v>
       </c>
       <c r="F18">
         <v>-2.3329367469198801E-2</v>
@@ -1675,12 +1623,12 @@
         <v>2.4360746692572999</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C19">
         <v>8</v>
@@ -1688,8 +1636,9 @@
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19">
-        <v>200</v>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>200 mg/vg</v>
       </c>
       <c r="F19">
         <v>-2.3329367469198801E-2</v>
@@ -1716,12 +1665,12 @@
         <v>0.99711443044647396</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>9</v>
@@ -1729,8 +1678,9 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20">
-        <v>200</v>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>200 mg/vg</v>
       </c>
       <c r="F20">
         <v>0.113036116867661</v>
@@ -1757,12 +1707,12 @@
         <v>1.3267368016116801</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>9</v>
@@ -1770,8 +1720,9 @@
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21">
-        <v>200</v>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>200 mg/vg</v>
       </c>
       <c r="F21">
         <v>0.113036116867661</v>
@@ -1798,12 +1749,12 @@
         <v>0.94017525666063295</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1811,8 +1762,9 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22">
-        <v>200</v>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>200 mg/vg</v>
       </c>
       <c r="F22">
         <v>-0.61697315546572196</v>
@@ -1839,12 +1791,12 @@
         <v>3.7513046151625802</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -1852,8 +1804,9 @@
       <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23">
-        <v>200</v>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>200 mg/vg</v>
       </c>
       <c r="F23">
         <v>-0.61697315546572196</v>
@@ -1880,12 +1833,12 @@
         <v>2.2751783300610899</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C24">
         <v>11</v>
@@ -1893,8 +1846,8 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24">
-        <v>300</v>
+      <c r="E24" t="s">
+        <v>48</v>
       </c>
       <c r="F24">
         <v>-1.21479800370346</v>
@@ -1921,12 +1874,12 @@
         <v>0.45342033227610901</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C25">
         <v>11</v>
@@ -1934,8 +1887,8 @@
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25">
-        <v>300</v>
+      <c r="E25" t="s">
+        <v>48</v>
       </c>
       <c r="F25">
         <v>-1.21479800370346</v>
@@ -1962,12 +1915,12 @@
         <v>1.1869910063837901</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -1975,8 +1928,8 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26">
-        <v>300</v>
+      <c r="E26" t="s">
+        <v>48</v>
       </c>
       <c r="F26">
         <v>-0.36746395712998903</v>
@@ -2003,12 +1956,12 @@
         <v>2.8807753991018101</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C27">
         <v>12</v>
@@ -2016,8 +1969,8 @@
       <c r="D27">
         <v>2</v>
       </c>
-      <c r="E27">
-        <v>300</v>
+      <c r="E27" t="s">
+        <v>48</v>
       </c>
       <c r="F27">
         <v>-0.36746395712998903</v>
@@ -2044,12 +1997,12 @@
         <v>2.3853937329262598</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>13</v>
@@ -2057,8 +2010,8 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28">
-        <v>300</v>
+      <c r="E28" t="s">
+        <v>48</v>
       </c>
       <c r="F28">
         <v>1.4413639146153201</v>
@@ -2085,12 +2038,12 @@
         <v>0.76408650923015697</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>13</v>
@@ -2098,8 +2051,8 @@
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="E29">
-        <v>300</v>
+      <c r="E29" t="s">
+        <v>48</v>
       </c>
       <c r="F29">
         <v>1.4413639146153201</v>
@@ -2126,12 +2079,12 @@
         <v>0.460664510491339</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <v>14</v>
@@ -2139,8 +2092,8 @@
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30">
-        <v>300</v>
+      <c r="E30" t="s">
+        <v>48</v>
       </c>
       <c r="F30">
         <v>-0.14882776237928</v>
@@ -2167,12 +2120,12 @@
         <v>1.5854333274249699</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>14</v>
@@ -2180,8 +2133,8 @@
       <c r="D31">
         <v>2</v>
       </c>
-      <c r="E31">
-        <v>300</v>
+      <c r="E31" t="s">
+        <v>48</v>
       </c>
       <c r="F31">
         <v>-0.14882776237928</v>
@@ -2208,12 +2161,12 @@
         <v>-0.35526439379382102</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>15</v>
@@ -2221,8 +2174,8 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32">
-        <v>300</v>
+      <c r="E32" t="s">
+        <v>48</v>
       </c>
       <c r="F32">
         <v>0.65506758960002298</v>
@@ -2249,12 +2202,12 @@
         <v>0.855619832489799</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C33">
         <v>15</v>
@@ -2262,8 +2215,8 @@
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="E33">
-        <v>300</v>
+      <c r="E33" t="s">
+        <v>48</v>
       </c>
       <c r="F33">
         <v>0.65506758960002298</v>
@@ -2290,12 +2243,12 @@
         <v>1.20718795884958</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C34">
         <v>16</v>
@@ -2303,6 +2256,7 @@
       <c r="D34">
         <v>1</v>
       </c>
+      <c r="E34"/>
       <c r="F34">
         <v>-0.31095282395058998</v>
       </c>
@@ -2328,12 +2282,12 @@
         <v>4.41803553160302</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C35">
         <v>16</v>
@@ -2341,6 +2295,7 @@
       <c r="D35">
         <v>2</v>
       </c>
+      <c r="E35"/>
       <c r="F35">
         <v>-0.31095282395058998</v>
       </c>
@@ -2366,12 +2321,12 @@
         <v>5.9019711311107397</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C36">
         <v>17</v>
@@ -2379,6 +2334,7 @@
       <c r="D36">
         <v>1</v>
       </c>
+      <c r="E36"/>
       <c r="F36">
         <v>0.29891293597051999</v>
       </c>
@@ -2404,12 +2360,12 @@
         <v>5.2721501053481399</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C37">
         <v>17</v>
@@ -2417,6 +2373,7 @@
       <c r="D37">
         <v>2</v>
       </c>
+      <c r="E37"/>
       <c r="F37">
         <v>0.29891293597051999</v>
       </c>
@@ -2442,12 +2399,12 @@
         <v>6.4712517188076397</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C38">
         <v>18</v>
@@ -2455,6 +2412,7 @@
       <c r="D38">
         <v>1</v>
       </c>
+      <c r="E38"/>
       <c r="F38">
         <v>-1.12050147779026</v>
       </c>
@@ -2480,12 +2438,12 @@
         <v>4.7839858734778904</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C39">
         <v>18</v>
@@ -2493,6 +2451,7 @@
       <c r="D39">
         <v>2</v>
       </c>
+      <c r="E39"/>
       <c r="F39">
         <v>-1.12050147779026</v>
       </c>
@@ -2518,12 +2477,12 @@
         <v>6.2669370673863902</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C40">
         <v>19</v>
@@ -2531,6 +2490,7 @@
       <c r="D40">
         <v>1</v>
       </c>
+      <c r="E40"/>
       <c r="F40">
         <v>0.40455689976052001</v>
       </c>
@@ -2556,12 +2516,12 @@
         <v>4.5679683537751101</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C41">
         <v>19</v>
@@ -2569,6 +2529,7 @@
       <c r="D41">
         <v>2</v>
       </c>
+      <c r="E41"/>
       <c r="F41">
         <v>0.40455689976052001</v>
       </c>
@@ -2594,12 +2555,12 @@
         <v>7.6611336627340796</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C42">
         <v>20</v>
@@ -2607,6 +2568,7 @@
       <c r="D42">
         <v>1</v>
       </c>
+      <c r="E42"/>
       <c r="F42">
         <v>-1.02109382908838</v>
       </c>
@@ -2632,12 +2594,12 @@
         <v>6.7753245799830797</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C43">
         <v>20</v>
@@ -2645,6 +2607,7 @@
       <c r="D43">
         <v>2</v>
       </c>
+      <c r="E43"/>
       <c r="F43">
         <v>-1.02109382908838</v>
       </c>
@@ -2670,12 +2633,12 @@
         <v>6.0668199864536101</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C44">
         <v>21</v>
@@ -2683,6 +2646,7 @@
       <c r="D44">
         <v>1</v>
       </c>
+      <c r="E44"/>
       <c r="F44">
         <v>0.36588553702114501</v>
       </c>
@@ -2708,12 +2672,12 @@
         <v>4.7904419404413403</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C45">
         <v>21</v>
@@ -2721,6 +2685,7 @@
       <c r="D45">
         <v>2</v>
       </c>
+      <c r="E45"/>
       <c r="F45">
         <v>0.36588553702114501</v>
       </c>
@@ -2746,12 +2711,12 @@
         <v>3.90456834936926</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C46">
         <v>22</v>
@@ -2759,6 +2724,7 @@
       <c r="D46">
         <v>1</v>
       </c>
+      <c r="E46"/>
       <c r="F46">
         <v>0.76795766603180404</v>
       </c>
@@ -2784,12 +2750,12 @@
         <v>4.5388158518432702</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C47">
         <v>22</v>
@@ -2797,6 +2763,7 @@
       <c r="D47">
         <v>2</v>
       </c>
+      <c r="E47"/>
       <c r="F47">
         <v>0.76795766603180404</v>
       </c>
@@ -2822,12 +2789,12 @@
         <v>4.57489638049167</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C48">
         <v>23</v>
@@ -2835,6 +2802,7 @@
       <c r="D48">
         <v>1</v>
       </c>
+      <c r="E48"/>
       <c r="F48">
         <v>-0.55848114046272301</v>
       </c>
@@ -2860,12 +2828,12 @@
         <v>4.5112837821820904</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C49">
         <v>23</v>
@@ -2873,6 +2841,7 @@
       <c r="D49">
         <v>2</v>
       </c>
+      <c r="E49"/>
       <c r="F49">
         <v>-0.55848114046272301</v>
       </c>
@@ -2898,12 +2867,12 @@
         <v>3.0635353258409102</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C50">
         <v>24</v>
@@ -2911,6 +2880,7 @@
       <c r="D50">
         <v>1</v>
       </c>
+      <c r="E50"/>
       <c r="F50">
         <v>0.47255251894759398</v>
       </c>
@@ -2936,12 +2906,12 @@
         <v>4.1754265829113804</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C51">
         <v>24</v>
@@ -2949,6 +2919,7 @@
       <c r="D51">
         <v>2</v>
       </c>
+      <c r="E51"/>
       <c r="F51">
         <v>0.47255251894759398</v>
       </c>
@@ -2974,12 +2945,12 @@
         <v>6.6082736656461503</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C52">
         <v>25</v>
@@ -2987,6 +2958,7 @@
       <c r="D52">
         <v>1</v>
       </c>
+      <c r="E52"/>
       <c r="F52">
         <v>-2.4950832984247602</v>
       </c>
@@ -3012,12 +2984,12 @@
         <v>5.9306926066945804</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C53">
         <v>25</v>
@@ -3025,6 +2997,7 @@
       <c r="D53">
         <v>2</v>
       </c>
+      <c r="E53"/>
       <c r="F53">
         <v>-2.4950832984247602</v>
       </c>
@@ -3050,12 +3023,12 @@
         <v>5.0390455708753796</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C54">
         <v>26</v>
@@ -3063,6 +3036,7 @@
       <c r="D54">
         <v>1</v>
       </c>
+      <c r="E54"/>
       <c r="F54">
         <v>1.5419594043740501</v>
       </c>
@@ -3088,12 +3062,12 @@
         <v>-0.26538304977348298</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C55">
         <v>26</v>
@@ -3101,6 +3075,7 @@
       <c r="D55">
         <v>2</v>
       </c>
+      <c r="E55"/>
       <c r="F55">
         <v>1.5419594043740501</v>
       </c>
@@ -3126,12 +3101,12 @@
         <v>0.64901390491817901</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C56">
         <v>27</v>
@@ -3139,6 +3114,7 @@
       <c r="D56">
         <v>1</v>
       </c>
+      <c r="E56"/>
       <c r="F56">
         <v>2.0024287958988798</v>
       </c>
@@ -3164,12 +3140,12 @@
         <v>-0.81729789730703795</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C57">
         <v>27</v>
@@ -3177,6 +3153,7 @@
       <c r="D57">
         <v>2</v>
       </c>
+      <c r="E57"/>
       <c r="F57">
         <v>2.0024287958988798</v>
       </c>
@@ -3202,12 +3179,12 @@
         <v>1.4333154532685199</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C58">
         <v>28</v>
@@ -3215,6 +3192,7 @@
       <c r="D58">
         <v>1</v>
       </c>
+      <c r="E58"/>
       <c r="F58">
         <v>0.38810422164820002</v>
       </c>
@@ -3240,12 +3218,12 @@
         <v>0.51831280576423699</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C59">
         <v>28</v>
@@ -3253,6 +3231,7 @@
       <c r="D59">
         <v>2</v>
       </c>
+      <c r="E59"/>
       <c r="F59">
         <v>0.38810422164820002</v>
       </c>
@@ -3278,12 +3257,12 @@
         <v>0.92580634524762695</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C60">
         <v>29</v>
@@ -3291,6 +3270,7 @@
       <c r="D60">
         <v>1</v>
       </c>
+      <c r="E60"/>
       <c r="F60">
         <v>-0.690821907340049</v>
       </c>
@@ -3316,12 +3296,12 @@
         <v>-1.1653680779945199</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C61">
         <v>29</v>
@@ -3329,6 +3309,7 @@
       <c r="D61">
         <v>2</v>
       </c>
+      <c r="E61"/>
       <c r="F61">
         <v>-0.690821907340049</v>
       </c>
@@ -3354,12 +3335,12 @@
         <v>-1.5640628300572601</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C62">
         <v>30</v>
@@ -3367,6 +3348,7 @@
       <c r="D62">
         <v>1</v>
       </c>
+      <c r="E62"/>
       <c r="F62">
         <v>-1.5672598117088401</v>
       </c>
@@ -3392,12 +3374,12 @@
         <v>-1.26253680496401</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B63" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C63">
         <v>30</v>
@@ -3405,6 +3387,7 @@
       <c r="D63">
         <v>2</v>
       </c>
+      <c r="E63"/>
       <c r="F63">
         <v>-1.5672598117088401</v>
       </c>
@@ -3431,7 +3414,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>